<commit_message>
update in 2nd testcase
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ALL_PAGES/END_TO_END/TC02_Verify_HOME_PDP_PLP_CATEGORY.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ALL_PAGES/END_TO_END/TC02_Verify_HOME_PDP_PLP_CATEGORY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Rohit\Automation\Demo\Kaman\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanProd\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD7BFA7-31BC-4931-B89B-6F5888FAA962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6235D7D-82FD-4258-BE81-E176C2CACBC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC02_Verify_HOME_PDP_PLP_CATEGO" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <t>TestCase</t>
   </si>
@@ -612,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -766,60 +766,48 @@
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
@@ -827,12 +815,42 @@
         <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -847,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1073,15 +1091,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1278,6 +1287,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
@@ -1288,14 +1306,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1312,4 +1322,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>